<commit_message>
Add daily log file
</commit_message>
<xml_diff>
--- a/utils/data/battery_info.xlsx
+++ b/utils/data/battery_info.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,6 +585,46 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-07-08</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>19:34:21</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Plugged</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>charged;</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>100</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>96%</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>